<commit_message>
feat: refactor upload API to follow SOLID architecture patterns
- Implement pipeline pattern with FileUploadOrchestrator for complex workflows
- Add factory pattern with UploadServiceFactory for dependency injection
- Create custom exception hierarchy (FileValidationException, UploadException)
- Extract validation logic into dedicated validators following SRP
- Update Excel service to use "Distribution" column name (aligned with template)
- Fix fund source data parsing to handle empty rows properly
- Simplify upload.py endpoint to focus only on coordination, delegate business logic to services

This refactoring maintains backward compatibility while establishing clean architectural patterns for future development.

🤖 Generated with [Claude Code](https://claude.ai/code)

Co-Authored-By: Claude <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/backend/tests/test_data/(Input Data) Fund A_Q1 2025 distribution data_v1.3.xlsx
+++ b/backend/tests/test_data/(Input Data) Fund A_Q1 2025 distribution data_v1.3.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="Fund Source Data" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Fund Source Data" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -637,7 +637,7 @@
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>Distribution Amount</t>
+          <t>Distribution</t>
         </is>
       </c>
     </row>

</xml_diff>